<commit_message>
Code (703A) should work in IAR 9 now. Changed startup.s file and path is IDE configuration. Removed not used files.
</commit_message>
<xml_diff>
--- a/Excel/u85b_module/amplitude_correction.xlsx
+++ b/Excel/u85b_module/amplitude_correction.xlsx
@@ -16,10 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
-  <si>
-    <t>dist</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="22">
   <si>
     <t>true phase</t>
   </si>
@@ -27,24 +24,6 @@
     <t>true phase, deg</t>
   </si>
   <si>
-    <t>measured 500</t>
-  </si>
-  <si>
-    <t>measured 300</t>
-  </si>
-  <si>
-    <t>measured 200</t>
-  </si>
-  <si>
-    <t>measured 100</t>
-  </si>
-  <si>
-    <t>measured 40</t>
-  </si>
-  <si>
-    <t>measured 700</t>
-  </si>
-  <si>
     <t>Grow</t>
   </si>
   <si>
@@ -79,6 +58,30 @@
   </si>
   <si>
     <t>800vsTrue</t>
+  </si>
+  <si>
+    <t>dist, mm</t>
+  </si>
+  <si>
+    <t>measured ampl. 700</t>
+  </si>
+  <si>
+    <t>measured ampl. 500</t>
+  </si>
+  <si>
+    <t>measured ampl. 300</t>
+  </si>
+  <si>
+    <t>measured ampl. 200</t>
+  </si>
+  <si>
+    <t>measured ampl. 100</t>
+  </si>
+  <si>
+    <t>measured ampl. 40</t>
+  </si>
+  <si>
+    <t>removed offset</t>
   </si>
 </sst>
 </file>
@@ -127,7 +130,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -135,6 +138,8 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -180,7 +185,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Лист1!$A$20:$A$32</c:f>
+              <c:f>Лист1!$A$19:$A$31</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -228,7 +233,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Лист1!$B$20:$B$32</c:f>
+              <c:f>Лист1!$B$19:$B$31</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -275,7 +280,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Лист1!$A$20:$A$32</c:f>
+              <c:f>Лист1!$A$19:$A$31</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -323,7 +328,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Лист1!$C$20:$C$32</c:f>
+              <c:f>Лист1!$C$19:$C$31</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -376,7 +381,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Лист1!$A$20:$A$32</c:f>
+              <c:f>Лист1!$A$19:$A$31</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -424,7 +429,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Лист1!$D$20:$D$32</c:f>
+              <c:f>Лист1!$D$19:$D$31</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="13"/>
@@ -477,11 +482,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="133225856"/>
-        <c:axId val="133204992"/>
+        <c:axId val="212712448"/>
+        <c:axId val="214090880"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="133225856"/>
+        <c:axId val="212712448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -491,12 +496,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="133204992"/>
+        <c:crossAx val="214090880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="133204992"/>
+        <c:axId val="214090880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -507,7 +512,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="133225856"/>
+        <c:crossAx val="212712448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -535,13 +540,13 @@
     <xdr:from>
       <xdr:col>11</xdr:col>
       <xdr:colOff>236220</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>15</xdr:row>
       <xdr:rowOff>140970</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
       <xdr:colOff>541020</xdr:colOff>
-      <xdr:row>45</xdr:row>
+      <xdr:row>44</xdr:row>
       <xdr:rowOff>129540</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -851,47 +856,48 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L54"/>
+  <dimension ref="A1:L53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D42" sqref="D42"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12.77734375" customWidth="1"/>
     <col min="2" max="2" width="14.77734375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="14.5546875" customWidth="1"/>
+    <col min="3" max="3" width="18" customWidth="1"/>
     <col min="4" max="4" width="17.6640625" customWidth="1"/>
     <col min="5" max="5" width="13.5546875" customWidth="1"/>
-    <col min="6" max="6" width="14.5546875" customWidth="1"/>
-    <col min="7" max="8" width="12.44140625" customWidth="1"/>
+    <col min="6" max="6" width="18.5546875" customWidth="1"/>
+    <col min="7" max="7" width="18.77734375" customWidth="1"/>
+    <col min="8" max="8" width="18.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="E1" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="F1" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="G1" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="H1" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
@@ -1002,659 +1008,667 @@
         <v>261.39999999999998</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>922</v>
-      </c>
-      <c r="B6" s="2">
-        <f>A6/2.561</f>
-        <v>360.01561889886761</v>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="C7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B8" s="2">
+        <f>B2</f>
+        <v>0</v>
+      </c>
+      <c r="C8" s="1">
+        <f t="shared" ref="C8:H11" si="1">C2-$B2</f>
+        <v>0</v>
+      </c>
+      <c r="D8" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E8" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F8" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G8" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="H8" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B9" s="2">
-        <f>B2</f>
-        <v>0</v>
+      <c r="B9" s="3">
+        <f>B3</f>
+        <v>89.808668488871533</v>
       </c>
       <c r="C9" s="1">
-        <f>C2-$B2</f>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>-11.508668488871535</v>
       </c>
       <c r="D9" s="3">
-        <f>D2-$B2</f>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>-5.0086684888715354</v>
       </c>
       <c r="E9" s="1">
-        <f>E2-$B2</f>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>1.6913315111284675</v>
       </c>
       <c r="F9" s="1">
-        <f>F2-$B2</f>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>5.1913315111284675</v>
       </c>
       <c r="G9" s="1">
-        <f>G2-$B2</f>
-        <v>1</v>
+        <f t="shared" si="1"/>
+        <v>7.8913315111284703</v>
       </c>
       <c r="H9" s="1">
-        <f>H2-$B2</f>
-        <v>1</v>
+        <f t="shared" si="1"/>
+        <v>10.39133151112847</v>
+      </c>
+      <c r="K9" s="1">
+        <f>C9-H9</f>
+        <v>-21.900000000000006</v>
+      </c>
+      <c r="L9" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B10" s="3">
-        <f t="shared" ref="B10:B12" si="1">B3</f>
-        <v>89.808668488871533</v>
+      <c r="B10" s="2">
+        <f>B4</f>
+        <v>179.61733697774307</v>
       </c>
       <c r="C10" s="1">
-        <f>C3-$B3</f>
-        <v>-11.508668488871535</v>
+        <f t="shared" si="1"/>
+        <v>2.3826630222569349</v>
       </c>
       <c r="D10" s="3">
-        <f t="shared" ref="D10:E12" si="2">D3-$B3</f>
-        <v>-5.0086684888715354</v>
+        <f t="shared" si="1"/>
+        <v>2.1826630222569463</v>
       </c>
       <c r="E10" s="1">
-        <f t="shared" si="2"/>
-        <v>1.6913315111284675</v>
+        <f t="shared" si="1"/>
+        <v>1.9826630222569293</v>
       </c>
       <c r="F10" s="1">
-        <f t="shared" ref="F10:G10" si="3">F3-$B3</f>
-        <v>5.1913315111284675</v>
+        <f t="shared" si="1"/>
+        <v>2.5826630222569236</v>
       </c>
       <c r="G10" s="1">
-        <f t="shared" si="3"/>
-        <v>7.8913315111284703</v>
+        <f t="shared" si="1"/>
+        <v>1.5826630222569236</v>
       </c>
       <c r="H10" s="1">
-        <f t="shared" ref="H10" si="4">H3-$B3</f>
-        <v>10.39133151112847</v>
-      </c>
-      <c r="K10" s="1">
-        <f>C10-H10</f>
-        <v>-21.900000000000006</v>
-      </c>
-      <c r="L10" t="s">
-        <v>9</v>
-      </c>
+        <f t="shared" si="1"/>
+        <v>1.3826630222569349</v>
+      </c>
+      <c r="K10" s="1"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B11" s="2">
-        <f t="shared" si="1"/>
-        <v>179.61733697774307</v>
+      <c r="B11" s="3">
+        <f>B5</f>
+        <v>269.81647793830535</v>
       </c>
       <c r="C11" s="1">
-        <f>C4-$B4</f>
-        <v>2.3826630222569349</v>
-      </c>
-      <c r="D11" s="3">
-        <f t="shared" si="2"/>
-        <v>2.1826630222569463</v>
+        <f t="shared" si="1"/>
+        <v>11.183522061694646</v>
+      </c>
+      <c r="D11" s="1">
+        <f t="shared" si="1"/>
+        <v>5.8835220616946344</v>
       </c>
       <c r="E11" s="1">
-        <f t="shared" si="2"/>
-        <v>1.9826630222569293</v>
+        <f t="shared" si="1"/>
+        <v>-0.11647793830536557</v>
       </c>
       <c r="F11" s="1">
-        <f t="shared" ref="F11:G11" si="5">F4-$B4</f>
-        <v>2.5826630222569236</v>
+        <f t="shared" si="1"/>
+        <v>-3.3164779383053542</v>
       </c>
       <c r="G11" s="1">
-        <f t="shared" si="5"/>
-        <v>1.5826630222569236</v>
+        <f t="shared" si="1"/>
+        <v>-6.4164779383053769</v>
       </c>
       <c r="H11" s="1">
-        <f t="shared" ref="H11" si="6">H4-$B4</f>
-        <v>1.3826630222569349</v>
-      </c>
-      <c r="K11" s="1"/>
+        <f t="shared" si="1"/>
+        <v>-8.4164779383053769</v>
+      </c>
+      <c r="K11" s="1">
+        <f t="shared" ref="K11" si="2">C11-H11</f>
+        <v>19.600000000000023</v>
+      </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B12" s="3">
-        <f t="shared" si="1"/>
-        <v>269.81647793830535</v>
-      </c>
-      <c r="C12" s="1">
-        <f>C5-$B5</f>
-        <v>11.183522061694646</v>
-      </c>
-      <c r="D12" s="1">
-        <f t="shared" si="2"/>
-        <v>5.8835220616946344</v>
-      </c>
-      <c r="E12" s="1">
-        <f t="shared" si="2"/>
-        <v>-0.11647793830536557</v>
-      </c>
-      <c r="F12" s="1">
-        <f t="shared" ref="F12:G12" si="7">F5-$B5</f>
-        <v>-3.3164779383053542</v>
-      </c>
-      <c r="G12" s="1">
-        <f t="shared" si="7"/>
-        <v>-6.4164779383053769</v>
-      </c>
-      <c r="H12" s="1">
-        <f t="shared" ref="H12" si="8">H5-$B5</f>
-        <v>-8.4164779383053769</v>
-      </c>
-      <c r="K12" s="1">
-        <f t="shared" ref="K11:K12" si="9">C12-H12</f>
-        <v>19.600000000000023</v>
-      </c>
+      <c r="C12" s="1"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="C13" s="1"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
+      <c r="D13" s="1"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="D14" s="1"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="D15" s="1"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>11</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E19" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>4</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E18" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>1200</v>
+      </c>
+      <c r="B19"/>
+      <c r="D19" s="4"/>
+      <c r="E19">
+        <v>296.10000000000002</v>
+      </c>
+      <c r="F19">
+        <f>E19-270</f>
+        <v>26.100000000000023</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20">
-        <v>1200</v>
+        <v>1100</v>
       </c>
       <c r="B20"/>
-      <c r="D20" s="4"/>
+      <c r="D20" s="4">
+        <v>66.400000000000006</v>
+      </c>
       <c r="E20">
-        <v>296.10000000000002</v>
+        <v>293.39999999999998</v>
       </c>
       <c r="F20">
-        <f>E20-270</f>
-        <v>26.100000000000023</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+        <f t="shared" ref="F20:F31" si="3">E20-270</f>
+        <v>23.399999999999977</v>
+      </c>
+      <c r="H20" s="4"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21">
-        <v>1100</v>
+        <v>1000</v>
       </c>
       <c r="B21"/>
+      <c r="C21">
+        <v>32.799999999999997</v>
+      </c>
       <c r="D21" s="4">
-        <v>66.400000000000006</v>
+        <v>69.3</v>
       </c>
       <c r="E21">
-        <v>293.39999999999998</v>
+        <v>291</v>
       </c>
       <c r="F21">
-        <f t="shared" ref="F21:F32" si="10">E21-270</f>
-        <v>23.399999999999977</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+        <f t="shared" si="3"/>
+        <v>21</v>
+      </c>
+      <c r="H21" s="4"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22">
-        <v>1000</v>
+        <v>900</v>
       </c>
       <c r="B22"/>
       <c r="C22">
-        <v>32.799999999999997</v>
+        <v>33.9</v>
       </c>
       <c r="D22" s="4">
-        <v>69.3</v>
+        <v>72.099999999999994</v>
       </c>
       <c r="E22">
-        <v>291</v>
+        <v>287.8</v>
       </c>
       <c r="F22">
-        <f t="shared" si="10"/>
-        <v>21</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A23">
-        <v>900</v>
-      </c>
-      <c r="B23"/>
-      <c r="C23">
-        <v>33.9</v>
-      </c>
-      <c r="D23" s="4">
-        <v>72.099999999999994</v>
-      </c>
-      <c r="E23">
-        <v>287.8</v>
+        <f t="shared" si="3"/>
+        <v>17.800000000000011</v>
+      </c>
+      <c r="H22" s="4"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A23" s="5">
+        <v>800</v>
+      </c>
+      <c r="B23" s="5">
+        <v>18.399999999999999</v>
+      </c>
+      <c r="C23" s="5">
+        <v>35</v>
+      </c>
+      <c r="D23" s="6">
+        <v>74.8</v>
+      </c>
+      <c r="E23" s="5">
+        <v>285</v>
       </c>
       <c r="F23">
-        <f t="shared" si="10"/>
-        <v>17.800000000000011</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A24" s="5">
-        <v>800</v>
-      </c>
-      <c r="B24" s="5">
-        <v>18.399999999999999</v>
-      </c>
-      <c r="C24" s="5">
-        <v>35</v>
-      </c>
-      <c r="D24" s="6">
-        <v>74.8</v>
-      </c>
-      <c r="E24" s="5">
-        <v>285</v>
+        <f t="shared" si="3"/>
+        <v>15</v>
+      </c>
+      <c r="H23" s="4"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>700</v>
+      </c>
+      <c r="B24">
+        <v>19.399999999999999</v>
+      </c>
+      <c r="C24">
+        <v>36.799999999999997</v>
+      </c>
+      <c r="D24" s="4">
+        <v>78.099999999999994</v>
+      </c>
+      <c r="E24">
+        <v>282</v>
       </c>
       <c r="F24">
-        <f t="shared" si="10"/>
-        <v>15</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+        <f t="shared" si="3"/>
+        <v>12</v>
+      </c>
+      <c r="H24" s="4"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25">
-        <v>700</v>
+        <v>600</v>
       </c>
       <c r="B25">
-        <v>19.399999999999999</v>
+        <v>20.399999999999999</v>
       </c>
       <c r="C25">
-        <v>36.799999999999997</v>
+        <v>39.1</v>
       </c>
       <c r="D25" s="4">
-        <v>78.099999999999994</v>
+        <v>81</v>
       </c>
       <c r="E25">
-        <v>282</v>
+        <v>278.7</v>
       </c>
       <c r="F25">
-        <f t="shared" si="10"/>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+        <f t="shared" si="3"/>
+        <v>8.6999999999999886</v>
+      </c>
+      <c r="H25" s="4"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26">
-        <v>600</v>
-      </c>
-      <c r="B26">
-        <v>20.399999999999999</v>
+        <v>500</v>
+      </c>
+      <c r="B26" s="8">
+        <v>21.5</v>
       </c>
       <c r="C26">
-        <v>39.1</v>
+        <v>41.3</v>
       </c>
       <c r="D26" s="4">
-        <v>81</v>
+        <v>84.3</v>
       </c>
       <c r="E26">
-        <v>278.7</v>
+        <v>275.60000000000002</v>
       </c>
       <c r="F26">
-        <f t="shared" si="10"/>
-        <v>8.6999999999999886</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+        <f t="shared" si="3"/>
+        <v>5.6000000000000227</v>
+      </c>
+      <c r="H26" s="4"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27">
-        <v>500</v>
-      </c>
-      <c r="B27">
-        <v>21.5</v>
-      </c>
-      <c r="C27">
-        <v>41.3</v>
+        <v>400</v>
+      </c>
+      <c r="B27" s="8">
+        <v>22.7</v>
+      </c>
+      <c r="C27" s="8">
+        <v>43.5</v>
       </c>
       <c r="D27" s="4">
-        <v>84.3</v>
-      </c>
-      <c r="E27">
-        <v>275.60000000000002</v>
+        <v>87.3</v>
+      </c>
+      <c r="E27" s="8">
+        <v>272.7</v>
       </c>
       <c r="F27">
-        <f t="shared" si="10"/>
-        <v>5.6000000000000227</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A28">
-        <v>400</v>
-      </c>
-      <c r="B28">
-        <v>22.7</v>
-      </c>
-      <c r="C28">
-        <v>43.5</v>
-      </c>
-      <c r="D28" s="4">
-        <v>87.3</v>
-      </c>
-      <c r="E28">
-        <v>272.7</v>
+        <f t="shared" si="3"/>
+        <v>2.6999999999999886</v>
+      </c>
+      <c r="H27" s="4"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A28" s="5">
+        <v>300</v>
+      </c>
+      <c r="B28" s="5">
+        <v>24</v>
+      </c>
+      <c r="C28" s="8">
+        <v>45.9</v>
+      </c>
+      <c r="D28" s="7">
+        <v>90.7</v>
+      </c>
+      <c r="E28" s="8">
+        <v>269.2</v>
       </c>
       <c r="F28">
-        <f t="shared" si="10"/>
-        <v>2.6999999999999886</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A29" s="5">
-        <v>300</v>
-      </c>
-      <c r="B29" s="5">
-        <v>24</v>
-      </c>
-      <c r="C29" s="5">
-        <v>45.9</v>
-      </c>
-      <c r="D29" s="6">
-        <v>90.7</v>
-      </c>
-      <c r="E29" s="5">
-        <v>269.2</v>
+        <f t="shared" si="3"/>
+        <v>-0.80000000000001137</v>
+      </c>
+      <c r="H28" s="4"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>200</v>
+      </c>
+      <c r="B29">
+        <v>25.7</v>
+      </c>
+      <c r="C29">
+        <v>48.7</v>
+      </c>
+      <c r="D29" s="4">
+        <v>94.2</v>
+      </c>
+      <c r="E29">
+        <v>266.3</v>
       </c>
       <c r="F29">
-        <f t="shared" si="10"/>
-        <v>-0.80000000000001137</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+        <f t="shared" si="3"/>
+        <v>-3.6999999999999886</v>
+      </c>
+      <c r="H29" s="4"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="B30">
-        <v>25.7</v>
+        <v>27.5</v>
       </c>
       <c r="C30">
-        <v>48.7</v>
+        <v>51.8</v>
       </c>
       <c r="D30" s="4">
-        <v>94.2</v>
+        <v>97.7</v>
       </c>
       <c r="E30">
-        <v>266.3</v>
+        <v>263.39999999999998</v>
       </c>
       <c r="F30">
-        <f t="shared" si="10"/>
-        <v>-3.6999999999999886</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+        <f t="shared" si="3"/>
+        <v>-6.6000000000000227</v>
+      </c>
+      <c r="H30" s="4"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31">
+        <v>40</v>
+      </c>
+      <c r="B31">
+        <v>28.3</v>
+      </c>
+      <c r="C31">
+        <v>54</v>
+      </c>
+      <c r="D31" s="4">
         <v>100</v>
       </c>
-      <c r="B31">
-        <v>27.5</v>
-      </c>
-      <c r="C31">
-        <v>51.8</v>
-      </c>
-      <c r="D31" s="4">
-        <v>97.7</v>
-      </c>
       <c r="E31">
-        <v>263.39999999999998</v>
+        <v>261.60000000000002</v>
       </c>
       <c r="F31">
-        <f t="shared" si="10"/>
-        <v>-6.6000000000000227</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A32">
-        <v>40</v>
-      </c>
-      <c r="B32">
-        <v>28.3</v>
-      </c>
-      <c r="C32">
-        <v>54</v>
-      </c>
-      <c r="D32" s="4">
-        <v>100</v>
-      </c>
-      <c r="E32">
-        <v>261.60000000000002</v>
-      </c>
-      <c r="F32">
-        <f t="shared" si="10"/>
+        <f t="shared" si="3"/>
         <v>-8.3999999999999773</v>
       </c>
+      <c r="H31" s="4"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B32"/>
+      <c r="D32" s="4"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B33"/>
       <c r="D33" s="4"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B34"/>
-      <c r="D34" s="4"/>
+      <c r="A34" t="s">
+        <v>7</v>
+      </c>
+      <c r="B34" s="4">
+        <f>B23-B31</f>
+        <v>-9.9000000000000021</v>
+      </c>
+      <c r="C34" s="4">
+        <f t="shared" ref="C34:E34" si="4">C23-C31</f>
+        <v>-19</v>
+      </c>
+      <c r="D34" s="4">
+        <f t="shared" si="4"/>
+        <v>-25.200000000000003</v>
+      </c>
+      <c r="E34" s="4">
+        <f t="shared" si="4"/>
+        <v>23.399999999999977</v>
+      </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="B35" s="4">
-        <f>B24-B32</f>
-        <v>-9.9000000000000021</v>
+        <f>B23-B28</f>
+        <v>-5.6000000000000014</v>
       </c>
       <c r="C35" s="4">
-        <f t="shared" ref="C35:E35" si="11">C24-C32</f>
-        <v>-19</v>
+        <f t="shared" ref="C35:E35" si="5">C23-C28</f>
+        <v>-10.899999999999999</v>
       </c>
       <c r="D35" s="4">
-        <f t="shared" si="11"/>
-        <v>-25.200000000000003</v>
+        <f t="shared" si="5"/>
+        <v>-15.900000000000006</v>
       </c>
       <c r="E35" s="4">
-        <f t="shared" si="11"/>
-        <v>23.399999999999977</v>
+        <f t="shared" si="5"/>
+        <v>15.800000000000011</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
+        <v>13</v>
+      </c>
+      <c r="B36" s="4">
+        <f>B23-22.5</f>
+        <v>-4.1000000000000014</v>
+      </c>
+      <c r="C36" s="4">
+        <f>C23-45</f>
+        <v>-10</v>
+      </c>
+      <c r="D36" s="4">
+        <f>D23-90</f>
+        <v>-15.200000000000003</v>
+      </c>
+      <c r="E36" s="4">
+        <f>E23-270</f>
         <v>15</v>
       </c>
-      <c r="B36" s="4">
-        <f>B24-B29</f>
-        <v>-5.6000000000000014</v>
-      </c>
-      <c r="C36" s="4">
-        <f t="shared" ref="C36:E36" si="12">C24-C29</f>
-        <v>-10.899999999999999</v>
-      </c>
-      <c r="D36" s="4">
-        <f t="shared" si="12"/>
-        <v>-15.900000000000006</v>
-      </c>
-      <c r="E36" s="4">
-        <f t="shared" si="12"/>
-        <v>15.800000000000011</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
-        <v>20</v>
-      </c>
-      <c r="B37" s="4">
-        <f>B24-22.5</f>
-        <v>-4.1000000000000014</v>
-      </c>
-      <c r="C37" s="4">
-        <f>C24-45</f>
-        <v>-10</v>
-      </c>
-      <c r="D37" s="4">
-        <f>D24-90</f>
-        <v>-15.200000000000003</v>
-      </c>
-      <c r="E37" s="4">
-        <f>E24-270</f>
-        <v>15</v>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>0</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C42" t="s">
+        <v>11</v>
+      </c>
+      <c r="D42" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
-        <v>1</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C43" t="s">
-        <v>18</v>
-      </c>
-      <c r="D43" t="s">
-        <v>19</v>
+      <c r="A43">
+        <v>0</v>
+      </c>
+      <c r="B43" s="1">
+        <v>0</v>
+      </c>
+      <c r="C43" s="4">
+        <f>SIN(A43/180*3.14)*16</f>
+        <v>0</v>
+      </c>
+      <c r="D43" s="4">
+        <f>C43*16</f>
+        <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44">
-        <v>0</v>
-      </c>
-      <c r="B44" s="1">
-        <v>0</v>
+        <v>22</v>
+      </c>
+      <c r="B44">
+        <v>5.6</v>
       </c>
       <c r="C44" s="4">
-        <f>SIN(A44/180*3.14)*16</f>
-        <v>0</v>
+        <f t="shared" ref="C44:C46" si="6">SIN(A44/180*3.14)</f>
+        <v>0.37442610287940581</v>
       </c>
       <c r="D44" s="4">
-        <f>C44*16</f>
-        <v>0</v>
+        <f t="shared" ref="D44:D46" si="7">C44*16</f>
+        <v>5.9908176460704929</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45">
-        <v>22</v>
+        <v>45</v>
       </c>
       <c r="B45">
-        <v>5.6</v>
+        <v>11</v>
       </c>
       <c r="C45" s="4">
-        <f t="shared" ref="C45:C47" si="13">SIN(A45/180*3.14)</f>
-        <v>0.37442610287940581</v>
+        <f t="shared" si="6"/>
+        <v>0.70682518110536596</v>
       </c>
       <c r="D45" s="4">
-        <f t="shared" ref="D45:D47" si="14">C45*16</f>
-        <v>5.9908176460704929</v>
+        <f t="shared" si="7"/>
+        <v>11.309202897685855</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46">
-        <v>45</v>
+        <v>90</v>
       </c>
       <c r="B46">
+        <v>16</v>
+      </c>
+      <c r="C46" s="4">
+        <f t="shared" si="6"/>
+        <v>0.99999968293183461</v>
+      </c>
+      <c r="D46" s="4">
+        <f t="shared" si="7"/>
+        <v>15.999994926909354</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>0</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C49" t="s">
         <v>11</v>
       </c>
-      <c r="C46" s="4">
-        <f t="shared" si="13"/>
-        <v>0.70682518110536596</v>
-      </c>
-      <c r="D46" s="4">
-        <f t="shared" si="14"/>
-        <v>11.309202897685855</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A47">
-        <v>90</v>
-      </c>
-      <c r="B47">
-        <v>16</v>
-      </c>
-      <c r="C47" s="4">
-        <f t="shared" si="13"/>
-        <v>0.99999968293183461</v>
-      </c>
-      <c r="D47" s="4">
-        <f t="shared" si="14"/>
-        <v>15.999994926909354</v>
+      <c r="D49" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A50" t="s">
-        <v>1</v>
-      </c>
-      <c r="B50" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C50" t="s">
-        <v>18</v>
-      </c>
-      <c r="D50" t="s">
-        <v>19</v>
+      <c r="A50">
+        <v>0</v>
+      </c>
+      <c r="B50" s="1">
+        <v>0</v>
+      </c>
+      <c r="C50" s="4">
+        <f>SIN(A50/180*3.14)*16</f>
+        <v>0</v>
+      </c>
+      <c r="D50" s="4">
+        <f>C50*15</f>
+        <v>0</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51">
-        <v>0</v>
-      </c>
-      <c r="B51" s="1">
-        <v>0</v>
+        <v>22</v>
+      </c>
+      <c r="B51">
+        <v>4</v>
       </c>
       <c r="C51" s="4">
-        <f>SIN(A51/180*3.14)*16</f>
-        <v>0</v>
+        <f t="shared" ref="C51:C53" si="8">SIN(A51/180*3.14)</f>
+        <v>0.37442610287940581</v>
       </c>
       <c r="D51" s="4">
-        <f>C51*15</f>
-        <v>0</v>
+        <f t="shared" ref="D51:D53" si="9">C51*15</f>
+        <v>5.6163915431910869</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52">
-        <v>22</v>
+        <v>45</v>
       </c>
       <c r="B52">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="C52" s="4">
-        <f t="shared" ref="C52:C54" si="15">SIN(A52/180*3.14)</f>
-        <v>0.37442610287940581</v>
+        <f t="shared" si="8"/>
+        <v>0.70682518110536596</v>
       </c>
       <c r="D52" s="4">
-        <f t="shared" ref="D52:D54" si="16">C52*15</f>
-        <v>5.6163915431910869</v>
+        <f t="shared" si="9"/>
+        <v>10.60237771658049</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53">
-        <v>45</v>
+        <v>90</v>
       </c>
       <c r="B53">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C53" s="4">
-        <f t="shared" si="15"/>
-        <v>0.70682518110536596</v>
+        <f t="shared" si="8"/>
+        <v>0.99999968293183461</v>
       </c>
       <c r="D53" s="4">
-        <f t="shared" si="16"/>
-        <v>10.60237771658049</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A54">
-        <v>90</v>
-      </c>
-      <c r="B54">
-        <v>15</v>
-      </c>
-      <c r="C54" s="4">
-        <f t="shared" si="15"/>
-        <v>0.99999968293183461</v>
-      </c>
-      <c r="D54" s="4">
-        <f t="shared" si="16"/>
+        <f t="shared" si="9"/>
         <v>14.999995243977519</v>
       </c>
     </row>

</xml_diff>